<commit_message>
Update FW and GPIO speed
</commit_message>
<xml_diff>
--- a/Scheme/Timers.xlsx
+++ b/Scheme/Timers.xlsx
@@ -411,7 +411,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Increase FFT speed & bug fixes
</commit_message>
<xml_diff>
--- a/Scheme/Timers.xlsx
+++ b/Scheme/Timers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>period</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>EEPROM/PERIPH</t>
+  </si>
+  <si>
+    <t>интервал, мс</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +467,7 @@
         <v>20000</v>
       </c>
       <c r="E3" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1">
         <v>1000</v>
@@ -520,7 +523,7 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="1"/>
-        <v>49999</v>
+        <v>9999</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
@@ -572,7 +575,7 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="3"/>
@@ -607,6 +610,35 @@
       </c>
       <c r="G10" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" ref="B12:D12" si="5">1000/B3</f>
+        <v>50</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="E12" s="1">
+        <f>1000/E3</f>
+        <v>10</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" ref="F12:G12" si="6">1000/F3</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="6"/>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prepare to new rf-unit
</commit_message>
<xml_diff>
--- a/Scheme/Timers.xlsx
+++ b/Scheme/Timers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -432,7 +432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -505,36 +507,36 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <f>200*1000*1000</f>
-        <v>200000000</v>
+        <f>240*1000*1000</f>
+        <v>240000000</v>
       </c>
       <c r="C4" s="4">
         <f>B4</f>
-        <v>200000000</v>
+        <v>240000000</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" ref="D4:I4" si="0">C4</f>
-        <v>200000000</v>
+        <v>240000000</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>200000000</v>
+        <v>240000000</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>200000000</v>
+        <v>240000000</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
-        <v>200000000</v>
+        <v>240000000</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>200000000</v>
+        <v>240000000</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="0"/>
-        <v>200000000</v>
+        <v>240000000</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -543,35 +545,35 @@
       </c>
       <c r="B5" s="2">
         <f>B4/(B6+1)/B3-1</f>
-        <v>49999</v>
+        <v>59999</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:F5" si="1">C4/(C6+1)/C3-1</f>
-        <v>9999</v>
+        <v>11999</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="1"/>
-        <v>9999</v>
+        <v>11999</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>999</v>
+        <v>1199</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" ref="G5:I5" si="2">G4/(G6+1)/G3-1</f>
-        <v>499</v>
+        <v>599</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="2"/>
-        <v>999</v>
+        <v>1199</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="2"/>
-        <v>999</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
implement wifi raw rle data transfer
</commit_message>
<xml_diff>
--- a/Scheme/Timers.xlsx
+++ b/Scheme/Timers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Develop\Projects\WOLF\Scheme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="1">
         <v>100</v>
@@ -545,7 +545,7 @@
       </c>
       <c r="B5" s="2">
         <f>B4/(B6+1)/B3-1</f>
-        <v>59999</v>
+        <v>1199</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:F5" si="1">C4/(C6+1)/C3-1</f>
@@ -611,7 +611,7 @@
       </c>
       <c r="B7" s="2">
         <f>B4/(B6+1)/(B5+1)</f>
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" ref="C7:F7" si="3">C4/(C6+1)/(C5+1)</f>
@@ -680,7 +680,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ref="B12:D12" si="5">1000/B3</f>
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
Start FFT overlap implementation
</commit_message>
<xml_diff>
--- a/Scheme/Timers.xlsx
+++ b/Scheme/Timers.xlsx
@@ -439,7 +439,7 @@
   <dimension ref="A2:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
         <v>1000</v>
       </c>
       <c r="C3" s="1">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D3" s="1">
         <v>20000</v>
@@ -566,7 +566,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:F5" si="1">C4/(C6+1)/C3-1</f>
-        <v>11999</v>
+        <v>1199</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
@@ -640,7 +640,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ref="C7:F7" si="4">C4/(C6+1)/(C5+1)</f>
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="4"/>
@@ -721,7 +721,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="7"/>

</xml_diff>